<commit_message>
Started 2019 modeller. Sync to laptop
</commit_message>
<xml_diff>
--- a/No mini meets.xlsx
+++ b/No mini meets.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tang-\Documents\Python Scripts\skynet2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9E7A80FD-3AFC-477E-BE09-B448E2D46A44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77192BA-E8AD-421A-88EF-D67D215CECF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276"/>
+    <workbookView xWindow="15345" yWindow="6585" windowWidth="15390" windowHeight="9615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nominimeets" sheetId="1" r:id="rId1"/>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1023,16 +1023,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="17.3984375" customWidth="1"/>
+    <col min="5" max="16" width="5.59765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.45">

</xml_diff>